<commit_message>
optimise the augment manager code now runs faster
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\EOY\CSVParser\CSVParser\bin\Debug\net5.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\EOY\Bullet++\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D8F54-F46E-43CB-8A90-515B01007275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C9077-50E0-4BC8-872B-B91F80E7A93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19298" yWindow="-1448" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentList" sheetId="1" r:id="rId1"/>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
augment levels, rich text for augment descriptions and some update to the UI
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\EOY\Bullet++\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C9077-50E0-4BC8-872B-B91F80E7A93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37E91FB-635A-414A-A78B-086D6AF4106A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19298" yWindow="-1448" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Id</t>
   </si>
@@ -38,11 +49,6 @@
   </si>
   <si>
     <t>Laser sight</t>
-  </si>
-  <si>
-    <t>+2 Bullets
-+10% Bullet Damage
-You get a red laser sight to improve your aim</t>
   </si>
   <si>
     <t>def OnAttached() { 
@@ -55,9 +61,6 @@
     <t>Under barrel rocket launcher</t>
   </si>
   <si>
-    <t>+2 Rockets</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Rocket", "maxClip", "Flat", 2);
 } </t>
@@ -66,9 +69,6 @@
     <t>Extra Grenades</t>
   </si>
   <si>
-    <t>+2 Grenades</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Grenade", "maxClip", "Flat", 2);
 } </t>
@@ -77,9 +77,6 @@
     <t>Extra Rockets</t>
   </si>
   <si>
-    <t>+3 Rockets</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Rocket", "maxClip", "Flat", 3);
 } </t>
@@ -88,9 +85,6 @@
     <t>Pocket Grenade</t>
   </si>
   <si>
-    <t>+1 Grenade</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Grenade", "maxClip", "Flat", 1);
 } </t>
@@ -99,34 +93,10 @@
     <t>Laser</t>
   </si>
   <si>
-    <t>+5 laser fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 3);
-AddModifier("Laser", "maxLaserLength", "Flat", 5);
-} </t>
-  </si>
-  <si>
     <t>Thick Laser</t>
   </si>
   <si>
-    <t>+ 2 Laser fuel
-+ Laser width
-+ Laser Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserWidth", "Flat", 0.03);
-AddModifier("Laser", "damage", "Flat", 3);
-} </t>
-  </si>
-  <si>
     <t>Bigger Bullets</t>
-  </si>
-  <si>
-    <t>+1 Bullet                                                                                                                                                                                                                                                    +50% Bullet Size                                                                                                                                                                                                                                               +1 Bullet Damage</t>
   </si>
   <si>
     <t xml:space="preserve">def OnAttached() { 
@@ -139,11 +109,214 @@
     <t>Extra Bullets</t>
   </si>
   <si>
-    <t>+3 Bullets</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Bullet", "maxClip", "Flat", 3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;10&lt;/color&gt;/20/40&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;10/&lt;color=#00d100&gt;20&lt;/color&gt;/40&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;10/20/&lt;color=#00d100&gt;40&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 4);
+AddModifier("Bullet", "damage", "PercentAdd", 0.2);
+} 
+def OnUpdate() { LaserSight(); }</t>
+  </si>
+  <si>
+    <t>def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 8);
+AddModifier("Bullet", "damage", "PercentAdd", 0.4);
+} 
+def OnUpdate() { LaserSight(); }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 8);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 4);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Grenade", "maxClip", "Flat", 4);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Grenade", "maxClip", "Flat", 8);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 6);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 12);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;3&lt;/color&gt;/6/12&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/4&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/&lt;color=#00d100&gt;6&lt;/color&gt;/12&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/6/&lt;color=#00d100&gt;12&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Laser Fuel</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt;  Laser Fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 2);
+AddModifier("Laser", "maxLaserLength", "Flat", 5);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 4);
+AddModifier("Laser", "maxLaserLength", "Flat", 5);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 8);
+AddModifier("Laser", "maxLaserLength", "Flat", 5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt; Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.5&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser Damage</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt;  Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt;  Laser Damage</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenades</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 2);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 0.5);
+AddModifier("Laser", "damage", "Flat", 0.5);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 4);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 1);
+AddModifier("Laser", "damage", "Flat", 1);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 8);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 2);
+AddModifier("Laser", "damage", "Flat", 2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/4&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt; Bullet Size
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/4&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt;  Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  BulletSize
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt;  Bullet Damage</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Size
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 2);
+AddModifier("Bullet", "size", "PercentAdd", 1);
+AddModifier("Bullet", "damage", "Flat", 2);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 4);
+AddModifier("Bullet", "size", "PercentAdd", 2);
+AddModifier("Bullet", "damage", "Flat", 4);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;3&lt;/color&gt;/6/12&lt;/color&gt;&lt;/b&gt; Bullets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/&lt;color=#00d100&gt;6&lt;/color&gt;/12&lt;/color&gt;&lt;/b&gt;  Bullets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 6);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/6/&lt;color=#00d100&gt;12&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 12);
 } </t>
   </si>
 </sst>
@@ -628,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -636,6 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,20 +1165,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" customWidth="1"/>
+    <col min="7" max="7" width="56.28515625" customWidth="1"/>
+    <col min="8" max="8" width="77.85546875" customWidth="1"/>
+    <col min="9" max="9" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,169 +1191,290 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change laser augment to + % instead of flat damage
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\EOY\Bullet++\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B5DB23-C29F-4941-B014-F76529CC8F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE666B-D324-4B24-ABA0-29FF7EE3318C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19298" yWindow="-1448" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentList" sheetId="1" r:id="rId1"/>
@@ -231,46 +231,10 @@
 } </t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt; Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.5&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser Damage</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt;  Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt;  Laser Damage</t>
-  </si>
-  <si>
     <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenades</t>
   </si>
   <si>
     <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 0.5);
-AddModifier("Laser", "damage", "Flat", 0.5);
-} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 4);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 1);
-AddModifier("Laser", "damage", "Flat", 1);
-} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 8);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 2);
-AddModifier("Laser", "damage", "Flat", 2);
-} </t>
   </si>
   <si>
     <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/4&lt;/color&gt;&lt;/b&gt; Bullets
@@ -402,6 +366,42 @@
   <si>
     <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/200&lt;/color&gt;%&lt;/b&gt; Damage
 &lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%&lt;/color&gt;&lt;/b&gt; Reload Time</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt; Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt; Laser Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 2);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 0.5);
+AddModifier("Laser", "damage", "PercentAdd", 0.5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt;  Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 4);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 1);
+AddModifier("Laser", "damage", "PercentAdd", 1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 8);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 2);
+AddModifier("Laser", "damage", "PercentAdd", 2);
+} </t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1303,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>21</v>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
         <v>35</v>
@@ -1478,7 +1478,7 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>28</v>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -1510,7 +1510,7 @@
         <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>47</v>
@@ -1527,25 +1527,25 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1559,25 +1559,25 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1591,25 +1591,25 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEC6AC0-7D29-4682-A64B-D767D1372047}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1649,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -1678,31 +1678,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="I2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1710,25 +1710,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J3" s="10"/>
     </row>

</xml_diff>

<commit_message>
-Added a bool which controls heat seeking behavior in rockets -added an augment which turns it on.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021\EOY\Bullet++\Assets\StreamingAssets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atwis\OneDrive\Documents\BulletPP\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B5DB23-C29F-4941-B014-F76529CC8F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B282C4E-F0A7-4620-BA0B-33DDFE191050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentList" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -402,6 +402,15 @@
   <si>
     <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/200&lt;/color&gt;%&lt;/b&gt; Damage
 &lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%&lt;/color&gt;&lt;/b&gt; Reload Time</t>
+  </si>
+  <si>
+    <t>Circuit seeking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 1);
+AddModifier("Rocket","heatSeeking","Flat",3);
+} </t>
   </si>
 </sst>
 </file>
@@ -1273,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,6 +1621,29 @@
         <v>65</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1622,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEC6AC0-7D29-4682-A64B-D767D1372047}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-Added Bouncing Blade stats -Added bouncing Blade augment
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atwis\OneDrive\Documents\BulletPP\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B282C4E-F0A7-4620-BA0B-33DDFE191050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586C0561-3FBC-43D6-B076-5B8CB5333D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>Id</t>
   </si>
@@ -410,6 +410,29 @@
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Rocket", "maxClip", "Flat", 1);
 AddModifier("Rocket","heatSeeking","Flat",3);
+} </t>
+  </si>
+  <si>
+    <t>Bouncing Blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {  
+AddModifier("BouncingBlade", "maxClip", "Flat", 1);
+AddModifier("BouncingBlade", "amountOfBounces", "Flat", 3);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {  
+AddModifier("BouncingBlade", "maxClip", "Flat", 1);
+AddModifier("BouncingBlade", "amountOfBounces", "Flat", 5);
+AddModifier("BouncingBlade","bounceAdditionDamage","Flat",0.1);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {  
+AddModifier("BouncingBlade", "maxClip", "Flat", 1);
+AddModifier("BouncingBlade", "amountOfBounces", "Flat", 7);
+AddModifier("BouncingBlade","bounceAdditionDamage","Flat",0.2);
 } </t>
   </si>
 </sst>
@@ -1282,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,6 +1665,29 @@
       </c>
       <c r="J11" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduced all index of augment list by 1
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atwis\OneDrive\Documents\BulletPP\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8748CC63-9C25-44CD-AC2A-DB2326D88ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14183422-96EB-4595-B436-820D6911191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentList" sheetId="1" r:id="rId1"/>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>102</v>
@@ -1912,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEC6AC0-7D29-4682-A64B-D767D1372047}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix bounce synergy bug
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -553,7 +553,7 @@
   </si>
   <si>
     <t xml:space="preserve">def OnAttached() { 
-AddModifier("Character", "damageOnBounces", "Flat", 0.1);
+AddModifier("Character", "damageOnBounce", "Flat", 0.1);
 } </t>
   </si>
   <si>
@@ -563,7 +563,7 @@
   <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Character", "extraBounces", "Flat", 1);
-AddModifier("Character", "damageOnBounces", "Flat", 0.15);
+AddModifier("Character", "damageOnBounce", "Flat", 0.15);
 } </t>
   </si>
   <si>

</xml_diff>

<commit_message>
- Added "Freshly forged Ammo" augment - Added "dashing" synergy
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Pictures\Liam's Work\Progamminig\BulletPP\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A72F1-E0E2-4E1E-B3B1-CA29A8DC308B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB513098-1956-4E91-A632-729A4A3D531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -698,15 +698,74 @@
 AddModifier("Rocket", "damage", "Flat", 0.75);
 } </t>
   </si>
+  <si>
+    <t>Dashing</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>icons/Dash.png</t>
+  </si>
+  <si>
+    <t>3,1, 5</t>
+  </si>
+  <si>
+    <t>Freshly Forged Ammo</t>
+  </si>
+  <si>
+    <t>icons/FreshAmmo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {   
+AddModifier("Character", "extraDamageAfterReload", "Flat", 0.5);
+AddModifier("Bullet", "maxClip", "Flat", 1);
+AddModifier("Grenade", "maxClip", "Flat",1);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {   
+AddModifier("Character", "extraDamageAfterReload", "Flat", 0.7);
+AddModifier("Bullet", "maxClip", "Flat", 1);
+AddModifier("Grenade", "maxClip", "Flat",2);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() {   
+AddModifier("Character", "extraDamageAfterReload", "Flat", 1);
+AddModifier("Bullet", "maxClip", "Flat", 2);
+AddModifier("Grenade", "maxClip", "Flat",2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50%&lt;/color&gt;/70%/100%&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;+1 Bullet, +1 Grenade&lt;/color&gt;/+1 Bullet, +2 Grenade/+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/&lt;color=#00d100&gt;70%&lt;/color&gt;/100%&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+1 Bullet, +1 Grenade/&lt;color=#00d100&gt;+1 Bullet, +2 Grenade&lt;/color&gt;/+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/70%/&lt;color=#00d100&gt;100%&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+1 Bullet, +1 Grenade/+1 Bullet, +2 Grenade/&lt;color=#00d100&gt;+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -729,9 +788,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,20 +1110,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="67.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="96" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="8" max="8" width="83" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" customWidth="1"/>
+    <col min="10" max="10" width="138.140625" customWidth="1"/>
     <col min="11" max="11" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1135,7 +1199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1154,7 +1218,7 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
@@ -1496,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
         <v>139</v>
@@ -1520,18 +1584,60 @@
         <v>145</v>
       </c>
     </row>
+    <row r="14" spans="1:11" ht="135">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -1725,6 +1831,23 @@
         <v>137</v>
       </c>
     </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-Added pause menu -Shop tells you when you can level up an augment
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AugmentList.xlsx
+++ b/Assets/StreamingAssets/AugmentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Pictures\Liam's Work\Progamminig\BulletPP\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB513098-1956-4E91-A632-729A4A3D531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66098E6C-6DB2-420A-A337-B15F8E0C7DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,25 +53,6 @@
     <t>icons/LotsofBullets.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;3&lt;/color&gt;/4/6&lt;/color&gt;&lt;/b&gt; Bullets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 3);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/&lt;color=#00d100&gt;4&lt;/color&gt;/6&lt;/color&gt;&lt;/b&gt; Bullets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 4);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/4/&lt;color=#00d100&gt;6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets</t>
-  </si>
-  <si>
     <t xml:space="preserve">def OnAttached() { 
 AddModifier("Bullet", "maxClip", "Flat", 6);
 } </t>
@@ -86,72 +67,12 @@
     <t>icons/BulletBounce.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Grenades
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Grenade", "maxClip", "Flat", 2);
-AddModifier("Grenade","amountOfBounces","Flat",1);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Grenades
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Grenade", "maxClip", "Flat", 3);
-AddModifier("Grenade","amountOfBounces","Flat",1);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenades
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Grenade", "maxClip", "Flat", 4);
-AddModifier("Grenade","amountOfBounces","Flat",2);
-} </t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
     <t>icons/Rocket.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/3&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.5&lt;/color&gt;/0.6/0.8&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 1);
-AddModifier("Rokcet", "radius","Flat", 0.5);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/3&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5&lt;color=#00d100&gt;0.6&lt;/color&gt;/0.8&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 2);
-AddModifier("Rokcet", "radius","Flat", 0.6);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;3&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/0.6/&lt;color=#00d100&gt;0.8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 3);
-AddModifier("Rokcet", "radius","Flat", 0.8);
-} </t>
-  </si>
-  <si>
     <t>Piercing Laser</t>
   </si>
   <si>
@@ -161,39 +82,6 @@
     <t>icons/DangerLaser.png</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Laser Charges
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/2.5/3.5&lt;/color&gt;&lt;/b&gt; Laser Size
-A powerful Laser to burn right through your enemies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserLength", "Flat", 2);
-} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Laser Charges
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;2.5&lt;/color&gt;/3.5&lt;/color&gt;&lt;/b&gt; Laser Size
-A powerful Laser to burn right through your enemies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 3);
-AddModifier("Laser", "maxLaserLength", "Flat", 2.5);
-} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Charges
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/2.5/&lt;color=#00d100&gt;3.5&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Size
-A powerful Laser to burn right through your enemies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 4);
-AddModifier("Laser", "maxLaserLength", "Flat", 3.5);
-} </t>
-  </si>
-  <si>
     <t>Laser sight</t>
   </si>
   <si>
@@ -203,42 +91,6 @@
     <t>icons/Cross.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;5&lt;/color&gt;/10/20&lt;/color&gt;%&lt;/b&gt; Bullet Damage
-You get a red laser sight to improve your aim</t>
-  </si>
-  <si>
-    <t>def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 2);
-AddModifier("Bullet", "damage", "PercentAdd", 0.05);
-} 
-def OnUpdate() { LaserSight(); }</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/&lt;color=#00d100&gt;10&lt;/color&gt;/20&lt;/color&gt;%&lt;/b&gt; Bullet Damage
-You get a red laser sight to improve your aim</t>
-  </si>
-  <si>
-    <t>def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 3);
-AddModifier("Bullet", "damage", "PercentAdd", 0.1);
-} 
-def OnUpdate() { LaserSight(); }</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/10/&lt;color=#00d100&gt;20&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Damage
-You get a red laser sight to improve your aim</t>
-  </si>
-  <si>
-    <t>def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 4);
-AddModifier("Bullet", "damage", "PercentAdd", 0.2);
-} 
-def OnUpdate() { LaserSight(); }</t>
-  </si>
-  <si>
     <t>Under barrel rocket launcher</t>
   </si>
   <si>
@@ -248,36 +100,6 @@
     <t>icons/RocketBlack.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.5&lt;/color&gt;/0.7/1&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 1);
-AddModifier("Rokcet", "damage","Flat", 0.5);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/&lt;color=#00d100&gt;0.7&lt;/color&gt;/1&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 1);
-AddModifier("Rokcet", "damage","Flat", 0.7);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/0.7/&lt;color=#00d100&gt;1&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 2);
-AddModifier("Rokcet", "damage","Flat", 1);
-} </t>
-  </si>
-  <si>
     <t>Bigger Bullets</t>
   </si>
   <si>
@@ -287,68 +109,10 @@
     <t>icons/BulletUpgrade.png</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/60/80&lt;/color&gt;%&lt;/b&gt; Bullet Size
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.4/0.6&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 2);
-AddModifier("Bullet", "size", "PercentAdd", 0.5);
-AddModifier("Bullet", "damage", "Flat", 0.3);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt;  Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;60&lt;/color&gt;/80&lt;/color&gt;%&lt;/b&gt;  BulletSize
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.3/&lt;color=#00d100&gt;0.4&lt;/color&gt;/0.6&lt;/color&gt;&lt;/b&gt;  Bullet Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 3);
-AddModifier("Bullet", "size", "PercentAdd", 0.6);
-AddModifier("Bullet", "damage", "Flat", 0.4);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/60/&lt;color=#00d100&gt;80&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Size
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.3/0.4/&lt;color=#00d100&gt;0.6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Bullet", "maxClip", "Flat", 4);
-AddModifier("Bullet", "size", "PercentAdd", 0.8);
-AddModifier("Bullet", "damage", "Flat", 0.6);
-} </t>
-  </si>
-  <si>
     <t>Value Pack</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/2&lt;/color&gt;&lt;/b&gt; Bullet
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/2&lt;/color&gt;&lt;/b&gt; Grenade
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser charge
-For when you just can't decide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 1);
-AddModifier("Laser", "maxClip", "Flat", 1);
-AddModifier("Bullet", "maxClip", "Flat", 1);
-AddModifier("Grenade", "maxClip", "Flat", 1);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Bullet
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Grenade
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Laser charge
-For when you just can't decide</t>
   </si>
   <si>
     <t xml:space="preserve">def OnAttached() { 
@@ -359,106 +123,13 @@
 } </t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullet
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenade
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser charge
-For when you just can't decide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Bullet", "maxClip", "Flat", 2);
-AddModifier("Grenade", "maxClip", "Flat", 2);
-} </t>
-  </si>
-  <si>
     <t>Thick Laser</t>
   </si>
   <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/4/8&lt;/color&gt;&lt;/b&gt; Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.2&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser Damage
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.1&lt;/color&gt;/0.2/0.3&lt;/color&gt;&lt;/b&gt; Travel Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 0.5);
-AddModifier("Laser", "damage", "Flat", 0.2);
-AddModifier("Laser", "travelTime", "Flat", 0.1);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;4&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt;  Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.5&lt;/color&gt;&lt;/b&gt;  Laser Damage
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.1/&lt;color=#00d100&gt;0.2&lt;/color&gt;/0.3&lt;/color&gt;&lt;/b&gt; Travel Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 1);
-AddModifier("Laser", "damage", "Flat", 0.3);
-AddModifier("Laser", "travelTime", "Flat", 0.2);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/4/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Width
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/0.3/&lt;color=#00d100&gt;0.5&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Damage
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.1/0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Travel Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Laser", "maxClip", "Flat", 2);
-AddModifier("Laser", "maxLaserWidth", "PercentAdd", 2);
-AddModifier("Laser", "damage", "Flat", 0.5);
-AddModifier("Laser", "travelTime", "Flat", 0.3);
-} </t>
-  </si>
-  <si>
     <t>Circuit Seeking Missiles</t>
   </si>
   <si>
     <t>0,3</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/2/3&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.2&lt;/color&gt;/0.3/0.4&lt;/color&gt;&lt;/b&gt; Rocket Damage
-Rockets you can recorrect after being fired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 1);
-AddModifier("Rocket","heatSeeking","Flat",3);
-AddModifier("Rocket","damage","Flat",0.2);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;2&lt;/color&gt;/3&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.4&lt;/color&gt;&lt;/b&gt; Rocket Damage
-Rockets you can recorrect after being fired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 2);
-AddModifier("Rocket","heatSeeking","Flat",3);
-AddModifier("Rocket","damage","Flat",0.3);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;2&lt;/color&gt;3&lt;/color&gt;&lt;/b&gt; Rocket
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/0.3/&lt;color=#00d100&gt;0.4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Damage
-Rockets you can recorrect after being fired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def OnAttached() { 
-AddModifier("Rocket", "maxClip", "Flat", 3);
-AddModifier("Rocket","heatSeeking","Flat",3);
-AddModifier("Rocket","damage","Flat",0.4);
-} </t>
   </si>
   <si>
     <t>Loose Saw Blade</t>
@@ -717,40 +388,369 @@
     <t>icons/FreshAmmo.png</t>
   </si>
   <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/6/&lt;color=#00d100&gt;8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/&lt;color=#00d100&gt;6&lt;/color&gt;/8&lt;/color&gt;&lt;/b&gt; Bullets</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;5&lt;/color&gt;/6/8&lt;/color&gt;&lt;/b&gt; Bullets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 8);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Grenade", "maxClip", "Flat", 4);
+AddModifier("Grenade","amountOfBounces","Flat",1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;4&lt;/color&gt;/5/7&lt;/color&gt;&lt;/b&gt; Grenades
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/&lt;color=#00d100&gt;5&lt;/color&gt;/7&lt;/color&gt;&lt;/b&gt; Grenades
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Grenade", "maxClip", "Flat", 5);
+AddModifier("Grenade","amountOfBounces","Flat",1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/5/&lt;color=#00d100&gt;7&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenades
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenade Bounces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Grenade", "maxClip", "Flat", 7);
+AddModifier("Grenade","amountOfBounces","Flat",2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.5&lt;/color&gt;/0.6/0.8&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 2);
+AddModifier("Rokcet", "radius","Flat", 0.5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5&lt;color=#00d100&gt;0.6&lt;/color&gt;/0.8&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 3);
+AddModifier("Rokcet", "radius","Flat", 0.6);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.5/0.6/&lt;color=#00d100&gt;0.8&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Explosion Radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 4);
+AddModifier("Rokcet", "radius","Flat", 0.8);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;3&lt;/color&gt;/4/5&lt;/color&gt;&lt;/b&gt; Laser Charges
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/2.5/3.5&lt;/color&gt;&lt;/b&gt; Laser Size
+A powerful Laser to burn right through your enemies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 3);
+AddModifier("Laser", "maxLaserLength", "Flat", 2);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/&lt;color=#00d100&gt;4&lt;/color&gt;/5&lt;/color&gt;&lt;/b&gt; Laser Charges
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;2.5&lt;/color&gt;/3.5&lt;/color&gt;&lt;/b&gt; Laser Size
+A powerful Laser to burn right through your enemies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 4);
+AddModifier("Laser", "maxLaserLength", "Flat", 2.5);
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/4/&lt;color=#00d100&gt;5&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Charges
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/2.5/&lt;color=#00d100&gt;3.5&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Size
+A powerful Laser to burn right through your enemies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 5);
+AddModifier("Laser", "maxLaserLength", "Flat", 3.5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;4&lt;/color&gt;/5/6&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;10&lt;/color&gt;/15/30&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 4);
+AddModifier("Bullet", "damage", "PercentAdd", 0.10);
+} 
+def OnUpdate() { LaserSight(); }</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/&lt;color=#00d100&gt;5&lt;/color&gt;/6&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;10/&lt;color=#00d100&gt;15&lt;/color&gt;/30&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 5);
+AddModifier("Bullet", "damage", "PercentAdd", 0.15);
+} 
+def OnUpdate() { LaserSight(); }</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/5/&lt;color=#00d100&gt;6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;10/15/&lt;color=#00d100&gt;30&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Damage
+You get a red laser sight to improve your aim</t>
+  </si>
+  <si>
+    <t>def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 6);
+AddModifier("Bullet", "damage", "PercentAdd", 0.3);
+} 
+def OnUpdate() { LaserSight(); }</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;5&lt;/color&gt;/7/10&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 2);
+AddModifier("Rokcet", "damage","Flat", 0.5);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/&lt;color=#00d100&gt;7&lt;/color&gt;/10&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 3);
+AddModifier("Rokcet", "damage","Flat", 0.7);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rockets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;5/7/&lt;color=#00d100&gt;10&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 4);
+AddModifier("Rokcet", "damage","Flat", 1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;4&lt;/color&gt;/5/6&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/60/80&lt;/color&gt;%&lt;/b&gt; Bullet Size
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.4/0.6&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 4);
+AddModifier("Bullet", "size", "PercentAdd", 0.5);
+AddModifier("Bullet", "damage", "Flat", 0.3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/&lt;color=#00d100&gt;5&lt;/color&gt;/6&lt;/color&gt;&lt;/b&gt;  Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;60&lt;/color&gt;/80&lt;/color&gt;%&lt;/b&gt;  BulletSize
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.3/&lt;color=#00d100&gt;0.4&lt;/color&gt;/0.6&lt;/color&gt;&lt;/b&gt;  Bullet Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 5);
+AddModifier("Bullet", "size", "PercentAdd", 0.7);
+AddModifier("Bullet", "damage", "Flat", 0.4);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;4/5/&lt;color=#00d100&gt;6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullets
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/60/&lt;color=#00d100&gt;80&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Bullet Size
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.3/0.4/&lt;color=#00d100&gt;0.6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullet Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Bullet", "maxClip", "Flat", 6);
+AddModifier("Bullet", "size", "PercentAdd", 0.8);
+AddModifier("Bullet", "damage", "Flat", 1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/3&lt;/color&gt;&lt;/b&gt; Bullet
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/3&lt;/color&gt;&lt;/b&gt; Grenade
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/&lt;color=#00d100&gt;1&lt;/color&gt;/2&lt;/color&gt;&lt;/b&gt; Laser charge
+For when you just can't decide</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/3&lt;/color&gt;&lt;/b&gt; Bullet
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/3&lt;/color&gt;&lt;/b&gt; Grenade
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;1&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser charge
+For when you just can't decide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 1);
+AddModifier("Laser", "maxClip", "Flat", 1);
+AddModifier("Bullet", "maxClip", "Flat", 3);
+AddModifier("Grenade", "maxClip", "Flat", 3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;3&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Bullet
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;3&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Grenade
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/1/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;1/2/&lt;color=#00d100&gt;2&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser charge
+For when you just can't decide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 2);
+AddModifier("Laser", "maxClip", "Flat", 2);
+AddModifier("Bullet", "maxClip", "Flat", 3);
+AddModifier("Grenade", "maxClip", "Flat", 3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;3&lt;/color&gt;/4/6&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50&lt;/color&gt;/100/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.2&lt;/color&gt;/1/2&lt;/color&gt;&lt;/b&gt; Laser Damage
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.1&lt;/color&gt;/0.2/0.3&lt;/color&gt;&lt;/b&gt; Travel Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 3);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 0.5);
+AddModifier("Laser", "damage", "Flat", 0.2);
+AddModifier("Laser", "travelTime", "Flat", 0.1);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/&lt;color=#00d100&gt;4&lt;/color&gt;/6&lt;/color&gt;&lt;/b&gt;  Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/&lt;color=#00d100&gt;100&lt;/color&gt;/200&lt;/color&gt;%&lt;/b&gt;  Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.5&lt;/color&gt;&lt;/b&gt;  Laser Damage
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.1/&lt;color=#00d100&gt;0.2&lt;/color&gt;/0.3&lt;/color&gt;&lt;/b&gt; Travel Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 4);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 1);
+AddModifier("Laser", "damage", "Flat", 0.3);
+AddModifier("Laser", "travelTime", "Flat", 0.2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;3/4/&lt;color=#00d100&gt;6&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Fuel
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50/100/&lt;color=#00d100&gt;200&lt;/color&gt;&lt;/color&gt;%&lt;/b&gt; Laser Width
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/0.3/&lt;color=#00d100&gt;0.5&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Laser Damage
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.1/0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Travel Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Laser", "maxClip", "Flat", 6);
+AddModifier("Laser", "maxLaserWidth", "PercentAdd", 2);
+AddModifier("Laser", "damage", "Flat", 0.5);
+AddModifier("Laser", "travelTime", "Flat", 0.3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;2&lt;/color&gt;/3/4&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;0.2&lt;/color&gt;/0.3/0.5&lt;/color&gt;&lt;/b&gt; Rocket Damage
+Rockets you can recorrect after being fired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 2);
+AddModifier("Rocket","heatSeeking","Flat",3);
+AddModifier("Rocket","damage","Flat",0.2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/&lt;color=#00d100&gt;3&lt;/color&gt;/4&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/&lt;color=#00d100&gt;0.3&lt;/color&gt;/0.5&lt;/color&gt;&lt;/b&gt; Rocket Damage
+Rockets you can recorrect after being fired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 3);
+AddModifier("Rocket","heatSeeking","Flat",3);
+AddModifier("Rocket","damage","Flat",0.3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;2/3/&lt;color=#00d100&gt;4&lt;/color&gt;3&lt;/color&gt;&lt;/b&gt; Rocket
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;0.2/0.3/&lt;color=#00d100&gt;0.4&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Rocket Damage
+Rockets you can recorrect after being fired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def OnAttached() { 
+AddModifier("Rocket", "maxClip", "Flat", 4);
+AddModifier("Rocket","heatSeeking","Flat",3);
+AddModifier("Rocket","damage","Flat",0.4);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50%&lt;/color&gt;/70%/100%&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;+2 Bullet, +2 Grenade&lt;/color&gt;/+3 Bullet, +4 Grenade/+5 Bullet, +4 Grenade&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
+  </si>
+  <si>
     <t xml:space="preserve">def OnAttached() {   
 AddModifier("Character", "extraDamageAfterReload", "Flat", 0.5);
-AddModifier("Bullet", "maxClip", "Flat", 1);
-AddModifier("Grenade", "maxClip", "Flat",1);
-} </t>
+AddModifier("Bullet", "maxClip", "Flat", 2);
+AddModifier("Grenade", "maxClip", "Flat",2);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/&lt;color=#00d100&gt;70%&lt;/color&gt;/100%&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+2 Bullet, +2 Grenade/&lt;color=#00d100&gt;+3 Bullet, +3 Grenade&lt;/color&gt;/+4 Bullet, +4 Grenade&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
   </si>
   <si>
     <t xml:space="preserve">def OnAttached() {   
 AddModifier("Character", "extraDamageAfterReload", "Flat", 0.7);
-AddModifier("Bullet", "maxClip", "Flat", 1);
-AddModifier("Grenade", "maxClip", "Flat",2);
-} </t>
+AddModifier("Bullet", "maxClip", "Flat", 3);
+AddModifier("Grenade", "maxClip", "Flat",3);
+} </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/70%/&lt;color=#00d100&gt;100%&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Damage increase
+&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+2 Bullet, +2 Grenade/+3 Bullet, +3 Grenade/&lt;color=#00d100&gt;+4 Bullet, +4 Grenade&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; 
+The first shot after a reload does way more damage.</t>
   </si>
   <si>
     <t xml:space="preserve">def OnAttached() {   
 AddModifier("Character", "extraDamageAfterReload", "Flat", 1);
-AddModifier("Bullet", "maxClip", "Flat", 2);
-AddModifier("Grenade", "maxClip", "Flat",2);
-} </t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;50%&lt;/color&gt;/70%/100%&lt;/color&gt;&lt;/b&gt; Damage increase
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;&lt;color=#00d100&gt;+1 Bullet, +1 Grenade&lt;/color&gt;/+1 Bullet, +2 Grenade/+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/b&gt; 
-The first shot after a reload does way more damage.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/&lt;color=#00d100&gt;70%&lt;/color&gt;/100%&lt;/color&gt;&lt;/b&gt; Damage increase
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+1 Bullet, +1 Grenade/&lt;color=#00d100&gt;+1 Bullet, +2 Grenade&lt;/color&gt;/+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/b&gt; 
-The first shot after a reload does way more damage.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;+&lt;color=#c5c5c5ff&gt;50%/70%/&lt;color=#00d100&gt;100%&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; Damage increase
-&lt;b&gt;+&lt;color=#c5c5c5ff&gt;+1 Bullet, +1 Grenade/+1 Bullet, +2 Grenade/&lt;color=#00d100&gt;+2 Bullet, +2 Grenade&lt;/color&gt;&lt;/color&gt;&lt;/b&gt; 
-The first shot after a reload does way more damage.</t>
+AddModifier("Bullet", "maxClip", "Flat", 4);
+AddModifier("Grenade", "maxClip", "Flat",4);
+} </t>
   </si>
 </sst>
 </file>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1164,7 +1164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="60">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1181,337 +1181,337 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="60">
+        <v>95</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="192" customHeight="1">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="171.75" customHeight="1">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="105">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="60">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="169.5" customHeight="1">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="165.75" customHeight="1">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="F9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="94.5" customHeight="1">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90.75" customHeight="1">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K11" t="s">
-        <v>91</v>
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="92.25" customHeight="1">
@@ -1519,34 +1519,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="J12" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="122.25" customHeight="1">
@@ -1554,34 +1554,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="135">
@@ -1589,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1598,25 +1598,25 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1679,34 +1679,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1714,28 +1714,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1743,28 +1743,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1772,34 +1772,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1807,28 +1807,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1836,16 +1836,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>